<commit_message>
EPBDS-4633 Enhanced testing tool: Add posibility to set precision property for custor result _res_.$Value$Step (10)
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/testmethod/DoubleDeltaTest.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/testmethod/DoubleDeltaTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t>num</t>
   </si>
@@ -114,12 +114,6 @@
     <t>_res_.$Value$Value1</t>
   </si>
   <si>
-    <t>_res_.$Value$Value2</t>
-  </si>
-  <si>
-    <t>_res_.$Value$Value3</t>
-  </si>
-  <si>
     <t>NUM</t>
   </si>
   <si>
@@ -130,17 +124,28 @@
   </si>
   <si>
     <t>RES3</t>
+  </si>
+  <si>
+    <t>_res_.$Value$Value3 (0)</t>
+  </si>
+  <si>
+    <t>Test geTestDouble geTestDoubleTest2</t>
+  </si>
+  <si>
+    <t>_res_ (2)</t>
+  </si>
+  <si>
+    <t>_res_.$Value$Value2 (1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="FFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -286,12 +291,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -313,29 +324,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -637,25 +649,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E36"/>
+  <dimension ref="B2:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="false"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="34"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
@@ -702,16 +714,16 @@
       <c r="C10" s="7"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
@@ -722,7 +734,7 @@
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
+      <c r="B14" s="35"/>
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -790,23 +802,23 @@
       <c r="D21" s="11"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="21" t="s">
         <v>22</v>
       </c>
     </row>
@@ -817,10 +829,10 @@
       <c r="C26" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -831,10 +843,10 @@
       <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="22" t="s">
         <v>28</v>
       </c>
     </row>
@@ -845,20 +857,20 @@
       <c r="C28" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="32" t="s">
@@ -867,51 +879,51 @@
       <c r="C31" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="35" t="n">
-        <v>41418.61695377315</v>
-      </c>
-      <c r="E31" s="34"/>
+      <c r="D31" s="30">
+        <v>41421.787674722225</v>
+      </c>
+      <c r="E31" s="28"/>
     </row>
     <row r="32" spans="2:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
-      <c r="C32" s="0" t="s">
+      <c r="C32" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="33" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E32" s="34"/>
+      <c r="D32" s="27">
+        <v>2</v>
+      </c>
+      <c r="E32" s="28"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" t="s">
         <v>31</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="E34" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>14</v>
       </c>
       <c r="C35" s="20" t="s">
@@ -938,7 +950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
         <v>15</v>
       </c>
@@ -952,7 +964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="20" t="s">
         <v>16</v>
       </c>
@@ -966,20 +978,84 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39">
-      <c r="B39" s="31"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="28"/>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="26"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="23"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="31"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="29"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="29"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="29">
+        <v>1</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="29"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="29">
+        <v>2</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="29"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="29">
+        <v>3</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="29"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="29">
+        <v>4</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>